<commit_message>
saved or moved or deleted some testfiles and examples
</commit_message>
<xml_diff>
--- a/inst/SPEED/speedtable_1k_500.xlsx
+++ b/inst/SPEED/speedtable_1k_500.xlsx
@@ -2,20 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcorrale\R\mysource\EJAM\inst\SPEED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B14C09B-43B4-4FE6-A896-1AE738F62563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3BF010-35FC-4FB6-850B-4930ED2B0EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18780" yWindow="3670" windowWidth="19690" windowHeight="13610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12220" yWindow="3000" windowWidth="19690" windowHeight="16860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="3" r:id="rId1"/>
     <sheet name="Chart2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="data" sheetId="1" r:id="rId3"/>
+    <sheet name="Chart3" sheetId="5" r:id="rId4"/>
+    <sheet name="blockcount" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>points</t>
   </si>
@@ -66,6 +68,66 @@
   <si>
     <t>blockspersite</t>
   </si>
+  <si>
+    <t>getblocks</t>
+  </si>
+  <si>
+    <t>doagg</t>
+  </si>
+  <si>
+    <t>within 10 miles</t>
+  </si>
+  <si>
+    <t>within 5 miles</t>
+  </si>
+  <si>
+    <t>within 3.1 miles (5km)</t>
+  </si>
+  <si>
+    <t>within 1 mile</t>
+  </si>
+  <si>
+    <t>Blocks near each FRS site on average</t>
+  </si>
+  <si>
+    <t>within 31 miles (50km)</t>
+  </si>
+  <si>
+    <t>Radius</t>
+  </si>
+  <si>
+    <t>10 miles</t>
+  </si>
+  <si>
+    <t>31 miles (50km)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  3.1 miles (5km)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  5 miles</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>bb</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>blocks</t>
+  </si>
+  <si>
+    <t>find nearby blocks</t>
+  </si>
+  <si>
+    <t>aggregate indicators, percentiles, etc.</t>
+  </si>
 </sst>
 </file>
 
@@ -76,7 +138,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,8 +161,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,6 +239,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -157,7 +265,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -197,12 +305,87 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -353,7 +536,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$6</c:f>
+              <c:f>data!$B$3:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -374,7 +557,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$3:$G$6</c:f>
+              <c:f>data!$G$3:$G$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -622,20 +805,23 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$B$11</c:f>
+              <c:f>data!$B$9:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3.1068560000000001</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -643,20 +829,23 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$8:$G$11</c:f>
+              <c:f>data!$G$9:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -703,7 +892,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$B$16</c:f>
+              <c:f>data!$B$15:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -724,7 +913,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$13:$G$16</c:f>
+              <c:f>data!$G$15:$G$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -782,20 +971,23 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$18:$B$21</c:f>
+              <c:f>data!$B$20:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3.1068560000000001</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -803,20 +995,23 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$18:$G$21</c:f>
+              <c:f>data!$G$20:$G$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>5.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3.2</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
@@ -1229,7 +1424,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$6</c:f>
+              <c:f>data!$B$3:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1250,7 +1445,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$3:$G$6</c:f>
+              <c:f>data!$G$3:$G$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1498,20 +1693,23 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$B$11</c:f>
+              <c:f>data!$B$9:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3.1068560000000001</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -1519,20 +1717,23 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$8:$G$11</c:f>
+              <c:f>data!$G$9:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -1579,7 +1780,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$B$16</c:f>
+              <c:f>data!$B$15:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1600,7 +1801,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$13:$G$16</c:f>
+              <c:f>data!$G$15:$G$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1923,6 +2124,857 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Finding who lives nearby scales well.</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Calculating</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> all indicators &amp; percentiles </a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US" baseline="0"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>needs optimization.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$C$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>find nearby blocks</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$B$30:$B$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$C$30:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-603B-44D7-A6A9-D5A2E46BC3AF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$D$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>aggregate indicators, percentiles, etc.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$B$30:$B$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$D$30:$D$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-603B-44D7-A6A9-D5A2E46BC3AF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="933592816"/>
+        <c:axId val="933591152"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="933592816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Miles</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="933591152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="933591152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="120"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="933592816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>#</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of blocks and residents vs radius</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>1, 3, 5, 10, 31 miles</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.34762295030860113"/>
+          <c:y val="0.20523476594046702"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.8655807490716099E-3"/>
+          <c:y val="1.8827828127873758E-2"/>
+          <c:w val="0.99096896853762528"/>
+          <c:h val="0.97234048714115617"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:bubbleChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>blockcount!$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>b</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>blockcount!$A$21:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>blockcount!$B$21:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>blockcount!$C$21:$C$25</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>127.3952</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>916.66660000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2032.0742</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6286.7215999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34763.597999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E482-4B7D-8C78-CFDF3DEF852E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:bubbleScale val="300"/>
+        <c:showNegBubbles val="0"/>
+        <c:axId val="690636944"/>
+        <c:axId val="690636112"/>
+      </c:bubbleChart>
+      <c:valAx>
+        <c:axId val="690636944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.1000000000000001"/>
+          <c:min val="0.9"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="690636112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="690636112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.1000000000000001"/>
+          <c:min val="0.9"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="690636944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2003,6 +3055,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3035,11 +4167,1051 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="269">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{01ABFC24-A85F-4EEA-AE54-7C5D0E523287}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="126" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3050,7 +5222,18 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{771EA786-CAAA-4877-9E1E-AB65E138D30B}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="94" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="126" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{531B9EA9-D6EB-49E0-A911-3B780BD968E5}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="108" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3061,7 +5244,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8660694" cy="6285324"/>
+    <xdr:ext cx="8663214" cy="6289524"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -3414,7 +5597,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8660694" cy="6285324"/>
+    <xdr:ext cx="8663214" cy="6289524"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -3699,6 +5882,94 @@
 </c:userShapes>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>376115</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9769</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>361461</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>165099</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6D75002-E5F7-6765-220D-7616377B603F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8660694" cy="6285324"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2E570F7-09F3-68F7-9E4A-356FAC1F0F38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E04C2DA1-EF8F-4E90-B733-8EC6D32CF1BE}" name="Table2" displayName="Table2" ref="B3:C8" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="B3:C8" xr:uid="{E04C2DA1-EF8F-4E90-B733-8EC6D32CF1BE}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:C8">
+    <sortCondition ref="B3:B8"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{051A410B-17F1-44BE-8303-6301A6E10192}" name="Blocks near each FRS site on average" dataDxfId="2" dataCellStyle="Comma"/>
+    <tableColumn id="2" xr3:uid="{A032CCFC-4ADE-4319-BF40-06B9200C8801}" name="Radius" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3710,44 +5981,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -3797,9 +6068,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -3855,188 +6126,166 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="11.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.08984375" style="4" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="9.54296875" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.08984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" customWidth="1"/>
+    <col min="10" max="10" width="14.453125" customWidth="1"/>
+    <col min="11" max="11" width="18.54296875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12.7265625" customWidth="1"/>
+    <col min="13" max="13" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4058,17 +6307,26 @@
       <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="M1" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>5000</v>
       </c>
@@ -4080,11 +6338,13 @@
       <c r="E2" s="20"/>
       <c r="F2" s="21"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="19"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
       <c r="J2" s="21"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="21"/>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>5000</v>
       </c>
@@ -4106,17 +6366,22 @@
       <c r="G3" s="6">
         <v>181</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3">
         <v>36</v>
       </c>
-      <c r="I3" s="4">
+      <c r="K3" s="4">
         <v>31433608</v>
       </c>
-      <c r="J3" s="4">
+      <c r="L3" s="30">
         <v>6286.7215999999999</v>
       </c>
+      <c r="M3" s="31" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>5000</v>
       </c>
@@ -4138,17 +6403,22 @@
       <c r="G4">
         <v>92</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4">
         <v>18</v>
       </c>
-      <c r="I4" s="4">
+      <c r="K4" s="4">
         <v>10160371</v>
       </c>
-      <c r="J4" s="4">
+      <c r="L4" s="30">
         <v>2032.0742</v>
       </c>
+      <c r="M4" s="31" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>5000</v>
       </c>
@@ -4170,17 +6440,22 @@
       <c r="G5">
         <v>72</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5">
         <v>14</v>
       </c>
-      <c r="I5" s="4">
+      <c r="K5" s="4">
         <v>4583333</v>
       </c>
-      <c r="J5" s="4">
+      <c r="L5" s="30">
         <v>916.66660000000002</v>
       </c>
+      <c r="M5" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5000</v>
       </c>
@@ -4202,483 +6477,992 @@
       <c r="G6">
         <v>50</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6">
         <v>10</v>
       </c>
-      <c r="I6" s="4">
+      <c r="K6" s="4">
         <v>636976</v>
       </c>
-      <c r="J6" s="4">
+      <c r="L6" s="30">
         <v>127.3952</v>
       </c>
+      <c r="M6" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="15">
-        <v>1000</v>
-      </c>
-      <c r="B7" s="7">
-        <v>31</v>
-      </c>
-      <c r="C7" s="4">
-        <v>30000.000000000004</v>
-      </c>
-      <c r="D7" s="4">
-        <v>500.00000000000006</v>
-      </c>
-      <c r="E7" s="10">
-        <v>8.3333333333333339</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-      <c r="G7" s="24">
-        <v>120</v>
-      </c>
-      <c r="H7">
-        <v>120</v>
-      </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
+    <row r="7" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="25">
+        <v>2000</v>
+      </c>
+      <c r="B7" s="25">
+        <v>5</v>
+      </c>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25">
+        <v>47</v>
+      </c>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <v>1000</v>
       </c>
-      <c r="B8">
-        <v>10</v>
+      <c r="B8" s="7">
+        <v>31</v>
       </c>
       <c r="C8" s="4">
-        <v>87666</v>
+        <v>30000.000000000004</v>
       </c>
       <c r="D8" s="4">
-        <v>1461</v>
-      </c>
-      <c r="E8">
-        <v>24</v>
+        <v>500.00000000000006</v>
+      </c>
+      <c r="E8" s="10">
+        <v>8.3333333333333339</v>
       </c>
       <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>41</v>
-      </c>
-      <c r="H8">
-        <v>41</v>
-      </c>
-      <c r="I8" s="4">
-        <v>6326239</v>
-      </c>
-      <c r="J8" s="4">
-        <v>6326</v>
+        <v>2</v>
+      </c>
+      <c r="G8" s="24">
+        <v>120</v>
+      </c>
+      <c r="H8" s="29">
+        <v>20</v>
+      </c>
+      <c r="I8" s="29">
+        <v>100</v>
+      </c>
+      <c r="J8">
+        <v>120</v>
+      </c>
+      <c r="K8" s="22">
+        <v>34763598</v>
+      </c>
+      <c r="L8" s="22">
+        <f>K8/A8</f>
+        <v>34763.597999999998</v>
+      </c>
+      <c r="M8" s="31" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
         <v>1000</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C9" s="4">
-        <v>157843</v>
+        <v>87666</v>
       </c>
       <c r="D9" s="4">
-        <v>2631</v>
+        <v>1461</v>
       </c>
       <c r="E9">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>23</v>
-      </c>
-      <c r="H9">
-        <v>23</v>
-      </c>
-      <c r="I9" s="4">
-        <v>2038999</v>
-      </c>
-      <c r="J9" s="4">
-        <v>2039</v>
+        <v>41</v>
+      </c>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9">
+        <v>41</v>
+      </c>
+      <c r="K9" s="4">
+        <v>6326239</v>
+      </c>
+      <c r="L9" s="4">
+        <v>6326</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="15">
         <v>1000</v>
       </c>
       <c r="B10">
-        <v>3.1068560000000001</v>
-      </c>
-      <c r="C10" s="4">
-        <v>231320</v>
-      </c>
-      <c r="D10" s="4">
-        <v>3855</v>
-      </c>
-      <c r="E10">
-        <v>64</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D10" s="4"/>
       <c r="G10">
+        <v>26</v>
+      </c>
+      <c r="H10" s="28">
+        <v>8</v>
+      </c>
+      <c r="I10" s="28">
         <v>16</v>
       </c>
-      <c r="H10">
-        <v>16</v>
-      </c>
-      <c r="I10" s="4">
-        <v>909619</v>
-      </c>
-      <c r="J10" s="4">
-        <v>910</v>
-      </c>
+      <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
         <v>1000</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C11" s="4">
-        <v>365450</v>
+        <v>157843</v>
       </c>
       <c r="D11" s="4">
-        <v>6091</v>
+        <v>2631</v>
       </c>
       <c r="E11">
-        <v>102</v>
+        <v>44</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
+        <v>23</v>
+      </c>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11">
+        <v>23</v>
+      </c>
+      <c r="K11" s="4">
+        <v>2038999</v>
+      </c>
+      <c r="L11" s="4">
+        <v>2039</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" s="15">
+        <v>1000</v>
+      </c>
+      <c r="B12">
+        <v>3.1068560000000001</v>
+      </c>
+      <c r="C12" s="4">
+        <v>231320</v>
+      </c>
+      <c r="D12" s="4">
+        <v>3855</v>
+      </c>
+      <c r="E12">
+        <v>64</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>16</v>
+      </c>
+      <c r="H12" s="28">
+        <v>7</v>
+      </c>
+      <c r="I12" s="28">
+        <v>6</v>
+      </c>
+      <c r="J12">
+        <v>16</v>
+      </c>
+      <c r="K12" s="4">
+        <v>909619</v>
+      </c>
+      <c r="L12" s="4">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" s="15">
+        <v>1000</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4">
+        <v>365450</v>
+      </c>
+      <c r="D13" s="4">
+        <v>6091</v>
+      </c>
+      <c r="E13">
+        <v>102</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
         <v>10</v>
       </c>
-      <c r="H11">
+      <c r="H13" s="28">
+        <v>6</v>
+      </c>
+      <c r="I13" s="28">
+        <v>2.5</v>
+      </c>
+      <c r="J13">
         <v>10</v>
       </c>
-      <c r="I11" s="4">
+      <c r="K13" s="4">
         <v>124260</v>
       </c>
-      <c r="J11" s="4">
+      <c r="L13" s="4">
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="16">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" s="16">
         <v>500</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B14" s="7">
         <v>31</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>500</v>
-      </c>
-      <c r="B13">
-        <v>10</v>
-      </c>
-      <c r="C13" s="4">
-        <v>55675</v>
-      </c>
-      <c r="D13" s="4">
-        <v>928</v>
-      </c>
-      <c r="E13">
-        <v>15</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>32</v>
-      </c>
-      <c r="H13">
-        <v>65</v>
-      </c>
-      <c r="I13" s="4">
-        <v>3166319</v>
-      </c>
-      <c r="J13" s="4">
-        <v>6333</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>500</v>
-      </c>
-      <c r="B14">
-        <v>5</v>
-      </c>
-      <c r="C14" s="4">
-        <v>107580</v>
-      </c>
-      <c r="D14" s="4">
-        <v>1793</v>
-      </c>
-      <c r="E14">
-        <v>30</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>17</v>
-      </c>
-      <c r="H14">
-        <v>33</v>
-      </c>
-      <c r="I14" s="4">
-        <v>1014213</v>
-      </c>
-      <c r="J14" s="4">
-        <v>2028</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>500</v>
       </c>
       <c r="B15">
-        <v>3.1068560000000001</v>
+        <v>10</v>
       </c>
       <c r="C15" s="4">
-        <v>160444</v>
+        <v>55675</v>
       </c>
       <c r="D15" s="4">
-        <v>2674</v>
+        <v>928</v>
       </c>
       <c r="E15">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
-        <v>11</v>
-      </c>
-      <c r="H15">
-        <v>22</v>
-      </c>
-      <c r="I15" s="4">
-        <v>454192</v>
-      </c>
-      <c r="J15" s="4">
-        <v>908</v>
+        <v>32</v>
+      </c>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15">
+        <v>65</v>
+      </c>
+      <c r="K15" s="4">
+        <v>3166319</v>
+      </c>
+      <c r="L15" s="4">
+        <v>6333</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>500</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C16" s="4">
-        <v>220465</v>
+        <v>107580</v>
       </c>
       <c r="D16" s="4">
-        <v>3674</v>
+        <v>1793</v>
       </c>
       <c r="E16">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16">
+        <v>17</v>
+      </c>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16">
+        <v>33</v>
+      </c>
+      <c r="K16" s="4">
+        <v>1014213</v>
+      </c>
+      <c r="L16" s="4">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>500</v>
+      </c>
+      <c r="B17">
+        <v>3.1068560000000001</v>
+      </c>
+      <c r="C17" s="4">
+        <v>160444</v>
+      </c>
+      <c r="D17" s="4">
+        <v>2674</v>
+      </c>
+      <c r="E17">
+        <v>45</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>11</v>
+      </c>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17">
+        <v>22</v>
+      </c>
+      <c r="K17" s="4">
+        <v>454192</v>
+      </c>
+      <c r="L17" s="4">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>500</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4">
+        <v>220465</v>
+      </c>
+      <c r="D18" s="4">
+        <v>3674</v>
+      </c>
+      <c r="E18">
+        <v>61</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
         <v>8</v>
       </c>
-      <c r="H16">
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18">
         <v>16</v>
       </c>
-      <c r="I16" s="4">
+      <c r="K18" s="4">
         <v>62209</v>
       </c>
-      <c r="J16" s="4">
+      <c r="L18" s="4">
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="15">
-        <v>100</v>
-      </c>
-      <c r="B17" s="7">
-        <v>31</v>
-      </c>
-      <c r="C17" s="4">
-        <v>22500</v>
-      </c>
-      <c r="D17" s="4">
-        <v>375</v>
-      </c>
-      <c r="E17" s="10">
-        <v>6.25</v>
-      </c>
-      <c r="F17" s="2">
-        <v>0.26666666666666666</v>
-      </c>
-      <c r="G17" s="24">
-        <v>16</v>
-      </c>
-      <c r="H17">
-        <v>160</v>
-      </c>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="15">
-        <v>100</v>
-      </c>
-      <c r="B18" s="16">
-        <v>10</v>
-      </c>
-      <c r="C18" s="22">
-        <v>61120</v>
-      </c>
-      <c r="D18" s="22">
-        <v>1018.6666666666666</v>
-      </c>
-      <c r="E18" s="22">
-        <v>16.977777777777778</v>
-      </c>
-      <c r="F18" s="23">
-        <v>9.6666666666666665E-2</v>
-      </c>
-      <c r="G18" s="16">
-        <v>5.8</v>
-      </c>
-      <c r="H18" s="16">
-        <v>58</v>
-      </c>
-      <c r="I18" s="8"/>
-      <c r="J18" s="7"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="15">
         <v>100</v>
       </c>
-      <c r="B19">
-        <v>5</v>
+      <c r="B19" s="7">
+        <v>31</v>
       </c>
       <c r="C19" s="4">
-        <v>90000</v>
+        <v>22500</v>
       </c>
       <c r="D19" s="4">
-        <v>1500</v>
+        <v>375</v>
       </c>
       <c r="E19" s="10">
-        <v>25</v>
+        <v>6.25</v>
       </c>
       <c r="F19" s="2">
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="G19">
-        <v>4</v>
-      </c>
-      <c r="H19" s="4">
-        <v>40</v>
-      </c>
-      <c r="I19" s="8"/>
-      <c r="J19" s="7"/>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="G19" s="24">
+        <v>16</v>
+      </c>
+      <c r="H19" s="28">
+        <v>2</v>
+      </c>
+      <c r="I19" s="28">
+        <v>14</v>
+      </c>
+      <c r="J19">
+        <v>160</v>
+      </c>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="15">
         <v>100</v>
       </c>
-      <c r="B20">
-        <v>3.1068560000000001</v>
-      </c>
-      <c r="C20" s="4">
-        <v>112500</v>
-      </c>
-      <c r="D20" s="4">
-        <v>1875</v>
-      </c>
-      <c r="E20" s="10">
-        <v>31.25</v>
-      </c>
-      <c r="F20" s="2">
-        <v>5.3333333333333337E-2</v>
-      </c>
-      <c r="G20">
-        <v>3.2</v>
-      </c>
-      <c r="H20" s="4">
-        <v>32</v>
-      </c>
-      <c r="I20" s="8"/>
-      <c r="J20" s="7"/>
+      <c r="B20" s="16">
+        <v>10</v>
+      </c>
+      <c r="C20" s="22">
+        <v>61120</v>
+      </c>
+      <c r="D20" s="22">
+        <v>1018.6666666666666</v>
+      </c>
+      <c r="E20" s="22">
+        <v>16.977777777777778</v>
+      </c>
+      <c r="F20" s="23">
+        <v>9.6666666666666665E-2</v>
+      </c>
+      <c r="G20" s="16">
+        <v>5.8</v>
+      </c>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="16">
+        <v>58</v>
+      </c>
+      <c r="K20" s="8"/>
+      <c r="L20" s="7"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="15">
         <v>100</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="16">
+        <v>6</v>
+      </c>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="16">
+        <v>4.5</v>
+      </c>
+      <c r="H21" s="28">
+        <v>0</v>
+      </c>
+      <c r="I21" s="28">
+        <v>3</v>
+      </c>
+      <c r="J21" s="16"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="7"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" s="15">
+        <v>100</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22" s="4">
+        <v>90000</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1500</v>
+      </c>
+      <c r="E22" s="10">
+        <v>25</v>
+      </c>
+      <c r="F22" s="2">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="G22">
+        <v>4</v>
+      </c>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="4">
+        <v>40</v>
+      </c>
+      <c r="K22" s="8"/>
+      <c r="L22" s="7"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" s="15">
+        <v>100</v>
+      </c>
+      <c r="B23">
+        <v>3.1068560000000001</v>
+      </c>
+      <c r="C23" s="4">
+        <v>112500</v>
+      </c>
+      <c r="D23" s="4">
+        <v>1875</v>
+      </c>
+      <c r="E23" s="10">
+        <v>31.25</v>
+      </c>
+      <c r="F23" s="2">
+        <v>5.3333333333333337E-2</v>
+      </c>
+      <c r="G23">
+        <v>3.2</v>
+      </c>
+      <c r="H23" s="28">
+        <v>0</v>
+      </c>
+      <c r="I23" s="28">
+        <v>2</v>
+      </c>
+      <c r="J23" s="4">
+        <v>32</v>
+      </c>
+      <c r="K23" s="8"/>
+      <c r="L23" s="7"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24" s="15">
+        <v>100</v>
+      </c>
+      <c r="B24">
         <v>1</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C24" s="4">
         <v>120000.00000000001</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D24" s="4">
         <v>2000.0000000000002</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E24" s="10">
         <v>33.333333333333336</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F24" s="2">
         <v>0.05</v>
       </c>
-      <c r="G21">
+      <c r="G24">
         <v>3</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H24" s="28">
+        <v>0</v>
+      </c>
+      <c r="I24" s="28">
+        <v>0</v>
+      </c>
+      <c r="J24" s="4">
         <v>29.999999999999996</v>
       </c>
-      <c r="I21" s="8"/>
-      <c r="J21" s="7"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="7"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C24" s="11">
-        <f>(A24/G24)*(3600)</f>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C27" s="11">
+        <f>(A27/G27)*(3600)</f>
         <v>0</v>
       </c>
-      <c r="D24" s="11">
-        <f>C24/60</f>
+      <c r="D27" s="11">
+        <f>C27/60</f>
         <v>0</v>
       </c>
-      <c r="E24" s="12">
-        <f t="shared" ref="E24" si="0">D24/60</f>
+      <c r="E27" s="12">
+        <f t="shared" ref="E27" si="0">D27/60</f>
         <v>0</v>
       </c>
-      <c r="F24" s="13">
-        <f t="shared" ref="F24" si="1">G24/60</f>
+      <c r="F27" s="13">
+        <f t="shared" ref="F27" si="1">G27/60</f>
         <v>0.05</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G27" s="14">
         <v>3</v>
       </c>
-      <c r="H24" s="11" t="e">
-        <f t="shared" ref="H24" si="2">1000/E24</f>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="11" t="e">
+        <f t="shared" ref="J27" si="2">1000/E27</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="K29"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A30" s="15">
+        <v>1000</v>
+      </c>
+      <c r="B30" s="7">
+        <v>31</v>
+      </c>
+      <c r="C30" s="36">
+        <v>20</v>
+      </c>
+      <c r="D30" s="36">
+        <v>100</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="K30"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A31" s="15">
+        <v>1000</v>
+      </c>
+      <c r="B31">
+        <v>6</v>
+      </c>
+      <c r="C31" s="37">
+        <v>8</v>
+      </c>
+      <c r="D31" s="37">
+        <v>16</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="K31"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A32" s="15">
+        <v>1000</v>
+      </c>
+      <c r="B32">
+        <v>3.1</v>
+      </c>
+      <c r="C32" s="37">
+        <v>7</v>
+      </c>
+      <c r="D32" s="37">
+        <v>6</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="K32"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A33" s="15">
+        <v>1000</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" s="37">
+        <v>6</v>
+      </c>
+      <c r="D33" s="37">
+        <v>2.5</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="K33"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A34" s="15">
+        <v>100</v>
+      </c>
+      <c r="B34" s="7">
+        <v>31</v>
+      </c>
+      <c r="C34" s="37">
+        <v>2</v>
+      </c>
+      <c r="D34" s="37">
+        <v>14</v>
+      </c>
+      <c r="E34" s="4"/>
+      <c r="K34"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A35" s="15">
+        <v>100</v>
+      </c>
+      <c r="B35" s="16">
+        <v>6</v>
+      </c>
+      <c r="C35" s="37">
+        <v>0</v>
+      </c>
+      <c r="D35" s="37">
+        <v>3</v>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="K35"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A36" s="15">
+        <v>100</v>
+      </c>
+      <c r="B36">
+        <v>3.1068560000000001</v>
+      </c>
+      <c r="C36" s="37">
+        <v>0</v>
+      </c>
+      <c r="D36" s="37">
+        <v>2</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="K36"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A37" s="15">
+        <v>100</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" s="37">
+        <v>0</v>
+      </c>
+      <c r="D37" s="37">
+        <v>0</v>
+      </c>
+      <c r="E37" s="4"/>
+      <c r="K37"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05FDA2F-433B-46D5-B645-EA9455E674AD}">
+  <dimension ref="A3:C25"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="22.453125" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="32">
+        <v>127.3952</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>3.1</v>
+      </c>
+      <c r="B5" s="32">
+        <v>916.66660000000002</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="32">
+        <v>2032.0742</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7" s="32">
+        <v>6286.7215999999999</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>31</v>
+      </c>
+      <c r="B8" s="34">
+        <v>34763.597999999998</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" s="32">
+        <v>127.3952</v>
+      </c>
+      <c r="C14" s="32">
+        <v>127.3952</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>3.1</v>
+      </c>
+      <c r="B15" s="32">
+        <v>916.66660000000002</v>
+      </c>
+      <c r="C15" s="32">
+        <v>916.66660000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" s="32">
+        <v>2032.0742</v>
+      </c>
+      <c r="C16" s="32">
+        <v>2032.0742</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17" s="32">
+        <v>6286.7215999999999</v>
+      </c>
+      <c r="C17" s="32">
+        <v>6286.7215999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>31</v>
+      </c>
+      <c r="B18" s="34">
+        <v>34763.597999999998</v>
+      </c>
+      <c r="C18" s="34">
+        <v>34763.597999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" s="32">
+        <v>1</v>
+      </c>
+      <c r="C21" s="32">
+        <v>127.3952</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="32">
+        <v>916.66660000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" s="32">
+        <v>2032.0742</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" s="32">
+        <v>6286.7215999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="34">
+        <v>34763.597999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
MOVED OR RENAMED SEVERAL FILES WITHIN inst folder - trying to clean up and shorten filenames paths
</commit_message>
<xml_diff>
--- a/inst/SPEED/speedtable_1k_500.xlsx
+++ b/inst/SPEED/speedtable_1k_500.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcorrale\R\mysource\EJAM\inst\SPEED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3BF010-35FC-4FB6-850B-4930ED2B0EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497DA746-1D2D-4CC4-B11F-D476C05D127F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12220" yWindow="3000" windowWidth="19690" windowHeight="16860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="3" r:id="rId1"/>
     <sheet name="Chart2" sheetId="2" r:id="rId2"/>
-    <sheet name="data" sheetId="1" r:id="rId3"/>
-    <sheet name="Chart3" sheetId="5" r:id="rId4"/>
-    <sheet name="blockcount" sheetId="4" r:id="rId5"/>
+    <sheet name="Chart3" sheetId="5" r:id="rId3"/>
+    <sheet name="data" sheetId="1" r:id="rId4"/>
+    <sheet name="Chart4" sheetId="6" r:id="rId5"/>
+    <sheet name="blockcount" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>points</t>
   </si>
@@ -128,6 +129,24 @@
   <si>
     <t>aggregate indicators, percentiles, etc.</t>
   </si>
+  <si>
+    <t>ratio expect last step</t>
+  </si>
+  <si>
+    <t>ratio actual last step</t>
+  </si>
+  <si>
+    <t xml:space="preserve">actual </t>
+  </si>
+  <si>
+    <t>expect if all earlier steps ^2</t>
+  </si>
+  <si>
+    <t>ratio expect if all prior steps ^2</t>
+  </si>
+  <si>
+    <t>ratio cum from 1 mile</t>
+  </si>
 </sst>
 </file>
 
@@ -138,7 +157,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,8 +214,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,8 +295,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -260,12 +310,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -307,14 +419,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -327,26 +431,42 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -384,6 +504,20 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2159,6 +2293,309 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>#</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of blocks and residents vs radius</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>1, 3, 5, 10, 31 miles</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.34762295030860113"/>
+          <c:y val="0.20523476594046702"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.8655807490716099E-3"/>
+          <c:y val="1.8827828127873758E-2"/>
+          <c:w val="0.99096896853762528"/>
+          <c:h val="0.97234048714115617"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:bubbleChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>blockcount!$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>b</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>blockcount!$A$21:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>blockcount!$B$21:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>blockcount!$C$21:$C$25</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>127.3952</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>916.66660000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2032.0742</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6286.7215999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34763.597999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E482-4B7D-8C78-CFDF3DEF852E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:bubbleScale val="300"/>
+        <c:showNegBubbles val="0"/>
+        <c:axId val="690636944"/>
+        <c:axId val="690636112"/>
+      </c:bubbleChart>
+      <c:valAx>
+        <c:axId val="690636944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.1000000000000001"/>
+          <c:min val="0.9"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="690636112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="690636112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.1000000000000001"/>
+          <c:min val="0.9"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="690636944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>Finding who lives nearby scales well.</a:t>
             </a:r>
           </a:p>
@@ -2672,7 +3109,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2693,7 +3130,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2706,23 +3143,9 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>#</a:t>
+              <a:rPr lang="en-US" sz="2800"/>
+              <a:t># of Census Blocks nearby, per FRS site</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> of blocks and residents vs radius</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>1, 3, 5, 10, 31 miles</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2730,8 +3153,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.34762295030860113"/>
-          <c:y val="0.20523476594046702"/>
+          <c:x val="1.77873486451832E-2"/>
+          <c:y val="2.3743580637547876E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2747,7 +3170,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2770,55 +3193,117 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.8655807490716099E-3"/>
-          <c:y val="1.8827828127873758E-2"/>
-          <c:w val="0.99096896853762528"/>
-          <c:h val="0.97234048714115617"/>
+          <c:x val="0.1163973504861487"/>
+          <c:y val="0.11934637890303749"/>
+          <c:w val="0.85119116004357409"/>
+          <c:h val="0.72292352862510734"/>
         </c:manualLayout>
       </c:layout>
-      <c:bubbleChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>blockcount!$B$20</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>b</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
-            <a:noFill/>
-            <a:ln>
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>blockcount!$A$21:$A$25</c:f>
+              <c:f>data!$B$2:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>3.1068560000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -2828,56 +3313,32 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>blockcount!$B$21:$B$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:bubbleSize>
-            <c:numRef>
-              <c:f>blockcount!$C$21:$C$25</c:f>
+              <c:f>data!$L$2:$L$6</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>127.3952</c:v>
+                  <c:v>34763.597999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>916.66660000000002</c:v>
+                  <c:v>6286.7215999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2032.0742</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6286.7215999999999</c:v>
+                  <c:v>916.66660000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>34763.597999999998</c:v>
+                  <c:v>127.3952</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:bubbleSize>
-          <c:bubble3D val="0"/>
+          </c:yVal>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E482-4B7D-8C78-CFDF3DEF852E}"/>
+              <c16:uniqueId val="{00000000-C31A-46CB-AD38-C10CE3FF5A5F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2889,42 +3350,185 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:bubbleScale val="300"/>
-        <c:showNegBubbles val="0"/>
-        <c:axId val="690636944"/>
-        <c:axId val="690636112"/>
-      </c:bubbleChart>
+        <c:axId val="2033772175"/>
+        <c:axId val="2033772591"/>
+      </c:scatterChart>
       <c:valAx>
-        <c:axId val="690636944"/>
+        <c:axId val="2033772175"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.1000000000000001"/>
-          <c:min val="0.9"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2400"/>
+                  <a:t>Within how many miles of the FRS site? (radius)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="690636112"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2033772591"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="690636112"/>
+        <c:axId val="2033772591"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.1000000000000001"/>
-          <c:min val="0.9"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="690636944"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2033772175"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2938,13 +3542,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -2972,6 +3569,7 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -3135,6 +3733,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4168,7 +4806,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="269">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4195,8 +4833,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4276,6 +4914,13 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -4286,6 +4931,13 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -4297,9 +4949,11 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -4317,6 +4971,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4329,10 +4986,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -4653,6 +5310,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -4673,7 +5341,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="269">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4700,8 +5368,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4781,13 +5449,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="75000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -4798,13 +5459,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="75000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -4816,11 +5470,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -4838,9 +5490,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4853,10 +5502,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -5177,6 +5826,49 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
@@ -5189,6 +5881,468 @@
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
@@ -5211,7 +6365,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{01ABFC24-A85F-4EEA-AE54-7C5D0E523287}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="126" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="113" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5222,7 +6376,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{771EA786-CAAA-4877-9E1E-AB65E138D30B}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="126" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="113" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5233,7 +6387,20 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{531B9EA9-D6EB-49E0-A911-3B780BD968E5}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="108" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="113" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{2D30832A-157F-404E-B7BB-E0148B2DC96B}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5244,7 +6411,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8663214" cy="6289524"/>
+    <xdr:ext cx="8665221" cy="6288186"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -5597,7 +6764,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8663214" cy="6289524"/>
+    <xdr:ext cx="8665221" cy="6288186"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -5884,6 +7051,39 @@
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8665221" cy="6288186"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2E570F7-09F3-68F7-9E4A-356FAC1F0F38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
@@ -5923,17 +7123,17 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8660694" cy="6285324"/>
+    <xdr:ext cx="8669364" cy="6296186"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2E570F7-09F3-68F7-9E4A-356FAC1F0F38}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5B3AA21-F3E7-D4FF-0AAB-A44ECCBAD595}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5956,15 +7156,835 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.72922</cdr:x>
+      <cdr:y>0.08568</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.97521</cdr:x>
+      <cdr:y>0.16467</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02123E6C-2E3C-8673-12BD-EACDDFDD910C}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="6321903" y="539468"/>
+          <a:ext cx="2132590" cy="497323"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>31 miles from 1 mill FRS sites is</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" u="sng"/>
+            <a:t>35 Billion </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>block-to-site distances!</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.21675</cdr:x>
+      <cdr:y>0.67797</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.35817</cdr:x>
+      <cdr:y>0.72638</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="Arrow: Curved Down 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58A34C16-5C4C-B598-6892-102C08E2CE09}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="20092680">
+          <a:off x="1879126" y="4268641"/>
+          <a:ext cx="1225975" cy="304799"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="curvedDownArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.17489</cdr:x>
+      <cdr:y>0.71066</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.22237</cdr:x>
+      <cdr:y>0.78255</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="Arrow: Curved Down 3">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90279E94-935B-BFFF-F70F-D11C4BCE42A6}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="20092680">
+          <a:off x="1516189" y="4474445"/>
+          <a:ext cx="411640" cy="452623"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="curvedDownArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.17015</cdr:x>
+      <cdr:y>0.66805</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.21293</cdr:x>
+      <cdr:y>0.71089</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2EA7456-0CC8-D8D3-6265-3D33BB1B2F3D}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1475112" y="4206173"/>
+          <a:ext cx="370885" cy="269734"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>2x</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.27421</cdr:x>
+      <cdr:y>0.62123</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.31699</cdr:x>
+      <cdr:y>0.64934</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="6" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{026CA2A8-BC69-9E44-3D49-F2B51353CCF3}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2377260" y="3911375"/>
+          <a:ext cx="370885" cy="177013"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>3x</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.2841</cdr:x>
+      <cdr:y>0.30572</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.8918</cdr:x>
+      <cdr:y>0.44657</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="7" name="Arrow: Curved Down 6">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE1391AF-3D98-43E1-8FF4-8697B72D0492}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="19457057">
+          <a:off x="2462958" y="1924851"/>
+          <a:ext cx="5268412" cy="886856"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="curvedDownArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.54062</cdr:x>
+      <cdr:y>0.25173</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.5834</cdr:x>
+      <cdr:y>0.27984</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="8" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5587237-E5F4-CFF8-FEDB-CE2C25C5C08F}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4686862" y="1584915"/>
+          <a:ext cx="370885" cy="177013"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>6x</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.1167</cdr:x>
+      <cdr:y>0.53153</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.35103</cdr:x>
+      <cdr:y>0.61052</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="9" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF0E0164-5433-8C16-3A3C-2A006076D7FE}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1011729" y="3346619"/>
+          <a:ext cx="2031438" cy="497323"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>5 miles from 1 mill. FRS sites is</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" u="sng"/>
+            <a:t>2 Billion </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>block-to-site distances</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.19932</cdr:x>
+      <cdr:y>0.5971</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.22363</cdr:x>
+      <cdr:y>0.72696</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76573DA1-9A31-9D44-04E8-B6C29939CE36}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1727987" y="3759425"/>
+          <a:ext cx="210730" cy="817633"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E04C2DA1-EF8F-4E90-B733-8EC6D32CF1BE}" name="Table2" displayName="Table2" ref="B3:C8" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E04C2DA1-EF8F-4E90-B733-8EC6D32CF1BE}" name="Table2" displayName="Table2" ref="B3:C8" totalsRowShown="0" dataDxfId="2">
   <autoFilter ref="B3:C8" xr:uid="{E04C2DA1-EF8F-4E90-B733-8EC6D32CF1BE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:C8">
     <sortCondition ref="B3:B8"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{051A410B-17F1-44BE-8303-6301A6E10192}" name="Blocks near each FRS site on average" dataDxfId="2" dataCellStyle="Comma"/>
-    <tableColumn id="2" xr3:uid="{A032CCFC-4ADE-4319-BF40-06B9200C8801}" name="Radius" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{051A410B-17F1-44BE-8303-6301A6E10192}" name="Blocks near each FRS site on average" dataDxfId="1" dataCellStyle="Comma"/>
+    <tableColumn id="2" xr3:uid="{A032CCFC-4ADE-4319-BF40-06B9200C8801}" name="Radius" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6269,23 +8289,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.08984375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" customWidth="1"/>
-    <col min="10" max="10" width="14.453125" customWidth="1"/>
-    <col min="11" max="11" width="18.54296875" style="4" customWidth="1"/>
-    <col min="12" max="12" width="12.7265625" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="37"/>
+    <col min="9" max="9" width="7" style="37" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1"/>
     <col min="13" max="13" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -6307,26 +8332,26 @@
       <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="39" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5000</v>
       </c>
@@ -6338,13 +8363,18 @@
       <c r="E2" s="20"/>
       <c r="F2" s="21"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
       <c r="J2" s="21"/>
       <c r="K2" s="19"/>
-      <c r="L2" s="21"/>
+      <c r="L2" s="44">
+        <v>34763.597999999998</v>
+      </c>
+      <c r="M2" s="45" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>5000</v>
       </c>
@@ -6366,22 +8396,22 @@
       <c r="G3" s="6">
         <v>181</v>
       </c>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
       <c r="J3">
         <v>36</v>
       </c>
       <c r="K3" s="4">
         <v>31433608</v>
       </c>
-      <c r="L3" s="30">
+      <c r="L3" s="40">
         <v>6286.7215999999999</v>
       </c>
-      <c r="M3" s="31" t="s">
+      <c r="M3" s="41" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5000</v>
       </c>
@@ -6403,22 +8433,22 @@
       <c r="G4">
         <v>92</v>
       </c>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
       <c r="J4">
         <v>18</v>
       </c>
       <c r="K4" s="4">
         <v>10160371</v>
       </c>
-      <c r="L4" s="30">
+      <c r="L4" s="40">
         <v>2032.0742</v>
       </c>
-      <c r="M4" s="31" t="s">
+      <c r="M4" s="41" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5000</v>
       </c>
@@ -6440,22 +8470,22 @@
       <c r="G5">
         <v>72</v>
       </c>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
       <c r="J5">
         <v>14</v>
       </c>
       <c r="K5" s="4">
         <v>4583333</v>
       </c>
-      <c r="L5" s="30">
+      <c r="L5" s="40">
         <v>916.66660000000002</v>
       </c>
-      <c r="M5" s="31" t="s">
+      <c r="M5" s="41" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5000</v>
       </c>
@@ -6477,22 +8507,22 @@
       <c r="G6">
         <v>50</v>
       </c>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
       <c r="J6">
         <v>10</v>
       </c>
       <c r="K6" s="4">
         <v>636976</v>
       </c>
-      <c r="L6" s="30">
+      <c r="L6" s="42">
         <v>127.3952</v>
       </c>
-      <c r="M6" s="31" t="s">
+      <c r="M6" s="43" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25">
         <v>2000</v>
       </c>
@@ -6506,13 +8536,13 @@
       <c r="G7" s="25">
         <v>47</v>
       </c>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
       <c r="J7" s="25"/>
       <c r="K7" s="26"/>
       <c r="L7" s="26"/>
     </row>
-    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>1000</v>
       </c>
@@ -6534,10 +8564,10 @@
       <c r="G8" s="24">
         <v>120</v>
       </c>
-      <c r="H8" s="29">
+      <c r="H8" s="32">
         <v>20</v>
       </c>
-      <c r="I8" s="29">
+      <c r="I8" s="32">
         <v>100</v>
       </c>
       <c r="J8">
@@ -6550,11 +8580,11 @@
         <f>K8/A8</f>
         <v>34763.597999999998</v>
       </c>
-      <c r="M8" s="31" t="s">
+      <c r="M8" s="27" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>1000</v>
       </c>
@@ -6576,8 +8606,8 @@
       <c r="G9">
         <v>41</v>
       </c>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
       <c r="J9">
         <v>41</v>
       </c>
@@ -6588,7 +8618,7 @@
         <v>6326</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>1000</v>
       </c>
@@ -6599,15 +8629,15 @@
       <c r="G10">
         <v>26</v>
       </c>
-      <c r="H10" s="28">
+      <c r="H10" s="33">
         <v>8</v>
       </c>
-      <c r="I10" s="28">
+      <c r="I10" s="33">
         <v>16</v>
       </c>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>1000</v>
       </c>
@@ -6629,8 +8659,8 @@
       <c r="G11">
         <v>23</v>
       </c>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
       <c r="J11">
         <v>23</v>
       </c>
@@ -6641,7 +8671,7 @@
         <v>2039</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>1000</v>
       </c>
@@ -6663,10 +8693,10 @@
       <c r="G12">
         <v>16</v>
       </c>
-      <c r="H12" s="28">
+      <c r="H12" s="33">
         <v>7</v>
       </c>
-      <c r="I12" s="28">
+      <c r="I12" s="33">
         <v>6</v>
       </c>
       <c r="J12">
@@ -6679,7 +8709,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>1000</v>
       </c>
@@ -6701,10 +8731,10 @@
       <c r="G13">
         <v>10</v>
       </c>
-      <c r="H13" s="28">
+      <c r="H13" s="33">
         <v>6</v>
       </c>
-      <c r="I13" s="28">
+      <c r="I13" s="33">
         <v>2.5</v>
       </c>
       <c r="J13">
@@ -6717,7 +8747,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
         <v>500</v>
       </c>
@@ -6729,13 +8759,13 @@
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
       <c r="G14" s="24"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
       <c r="J14" s="18"/>
       <c r="K14" s="17"/>
       <c r="L14" s="17"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>500</v>
       </c>
@@ -6757,8 +8787,8 @@
       <c r="G15">
         <v>32</v>
       </c>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
       <c r="J15">
         <v>65</v>
       </c>
@@ -6769,7 +8799,7 @@
         <v>6333</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>500</v>
       </c>
@@ -6791,8 +8821,8 @@
       <c r="G16">
         <v>17</v>
       </c>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
       <c r="J16">
         <v>33</v>
       </c>
@@ -6803,7 +8833,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>500</v>
       </c>
@@ -6825,8 +8855,8 @@
       <c r="G17">
         <v>11</v>
       </c>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
       <c r="J17">
         <v>22</v>
       </c>
@@ -6837,7 +8867,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>500</v>
       </c>
@@ -6859,8 +8889,8 @@
       <c r="G18">
         <v>8</v>
       </c>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
       <c r="J18">
         <v>16</v>
       </c>
@@ -6871,7 +8901,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>100</v>
       </c>
@@ -6893,10 +8923,10 @@
       <c r="G19" s="24">
         <v>16</v>
       </c>
-      <c r="H19" s="28">
+      <c r="H19" s="33">
         <v>2</v>
       </c>
-      <c r="I19" s="28">
+      <c r="I19" s="33">
         <v>14</v>
       </c>
       <c r="J19">
@@ -6905,7 +8935,7 @@
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>100</v>
       </c>
@@ -6927,15 +8957,15 @@
       <c r="G20" s="16">
         <v>5.8</v>
       </c>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
       <c r="J20" s="16">
         <v>58</v>
       </c>
       <c r="K20" s="8"/>
       <c r="L20" s="7"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>100</v>
       </c>
@@ -6949,17 +8979,17 @@
       <c r="G21" s="16">
         <v>4.5</v>
       </c>
-      <c r="H21" s="28">
+      <c r="H21" s="33">
         <v>0</v>
       </c>
-      <c r="I21" s="28">
+      <c r="I21" s="33">
         <v>3</v>
       </c>
       <c r="J21" s="16"/>
       <c r="K21" s="8"/>
       <c r="L21" s="7"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>100</v>
       </c>
@@ -6981,15 +9011,15 @@
       <c r="G22">
         <v>4</v>
       </c>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
       <c r="J22" s="4">
         <v>40</v>
       </c>
       <c r="K22" s="8"/>
       <c r="L22" s="7"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>100</v>
       </c>
@@ -7011,10 +9041,10 @@
       <c r="G23">
         <v>3.2</v>
       </c>
-      <c r="H23" s="28">
+      <c r="H23" s="33">
         <v>0</v>
       </c>
-      <c r="I23" s="28">
+      <c r="I23" s="33">
         <v>2</v>
       </c>
       <c r="J23" s="4">
@@ -7023,7 +9053,7 @@
       <c r="K23" s="8"/>
       <c r="L23" s="7"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>100</v>
       </c>
@@ -7045,10 +9075,10 @@
       <c r="G24">
         <v>3</v>
       </c>
-      <c r="H24" s="28">
+      <c r="H24" s="33">
         <v>0</v>
       </c>
-      <c r="I24" s="28">
+      <c r="I24" s="33">
         <v>0</v>
       </c>
       <c r="J24" s="4">
@@ -7057,15 +9087,15 @@
       <c r="K24" s="8"/>
       <c r="L24" s="7"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C27" s="11">
         <f>(A27/G27)*(3600)</f>
         <v>0</v>
@@ -7085,153 +9115,153 @@
       <c r="G27" s="14">
         <v>3</v>
       </c>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
       <c r="J27" s="11" t="e">
         <f t="shared" ref="J27" si="2">1000/E27</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B29" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="27" t="s">
+      <c r="C29" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="38" t="s">
+      <c r="D29" s="34" t="s">
         <v>29</v>
       </c>
       <c r="E29" s="4"/>
       <c r="K29"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>1000</v>
       </c>
       <c r="B30" s="7">
         <v>31</v>
       </c>
-      <c r="C30" s="36">
+      <c r="C30" s="32">
         <v>20</v>
       </c>
-      <c r="D30" s="36">
+      <c r="D30" s="32">
         <v>100</v>
       </c>
       <c r="E30" s="4"/>
       <c r="K30"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>1000</v>
       </c>
       <c r="B31">
         <v>6</v>
       </c>
-      <c r="C31" s="37">
+      <c r="C31" s="33">
         <v>8</v>
       </c>
-      <c r="D31" s="37">
+      <c r="D31" s="33">
         <v>16</v>
       </c>
       <c r="E31" s="4"/>
       <c r="K31"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>1000</v>
       </c>
       <c r="B32">
         <v>3.1</v>
       </c>
-      <c r="C32" s="37">
+      <c r="C32" s="33">
         <v>7</v>
       </c>
-      <c r="D32" s="37">
+      <c r="D32" s="33">
         <v>6</v>
       </c>
       <c r="E32" s="4"/>
       <c r="K32"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>1000</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
-      <c r="C33" s="37">
+      <c r="C33" s="33">
         <v>6</v>
       </c>
-      <c r="D33" s="37">
+      <c r="D33" s="33">
         <v>2.5</v>
       </c>
       <c r="E33" s="4"/>
       <c r="K33"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <v>100</v>
       </c>
       <c r="B34" s="7">
         <v>31</v>
       </c>
-      <c r="C34" s="37">
+      <c r="C34" s="33">
         <v>2</v>
       </c>
-      <c r="D34" s="37">
+      <c r="D34" s="33">
         <v>14</v>
       </c>
       <c r="E34" s="4"/>
       <c r="K34"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>100</v>
       </c>
       <c r="B35" s="16">
         <v>6</v>
       </c>
-      <c r="C35" s="37">
+      <c r="C35" s="33">
         <v>0</v>
       </c>
-      <c r="D35" s="37">
+      <c r="D35" s="33">
         <v>3</v>
       </c>
       <c r="E35" s="4"/>
       <c r="K35"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>100</v>
       </c>
       <c r="B36">
         <v>3.1068560000000001</v>
       </c>
-      <c r="C36" s="37">
+      <c r="C36" s="33">
         <v>0</v>
       </c>
-      <c r="D36" s="37">
+      <c r="D36" s="33">
         <v>2</v>
       </c>
       <c r="E36" s="4"/>
       <c r="K36"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>100</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
-      <c r="C37" s="37">
+      <c r="C37" s="33">
         <v>0</v>
       </c>
-      <c r="D37" s="37">
+      <c r="D37" s="33">
         <v>0</v>
       </c>
       <c r="E37" s="4"/>
@@ -7245,85 +9275,309 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05FDA2F-433B-46D5-B645-EA9455E674AD}">
-  <dimension ref="A3:C25"/>
+  <dimension ref="A2:M25"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C8"/>
+    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.453125" customWidth="1"/>
-    <col min="3" max="3" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="12" width="10.5703125" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="31" t="s">
         <v>18</v>
       </c>
+      <c r="D3" s="31"/>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="52" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="32">
+      <c r="B4" s="28">
         <v>127.3952</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="29" t="s">
         <v>15</v>
       </c>
+      <c r="D4" s="29"/>
+      <c r="E4">
+        <v>31</v>
+      </c>
+      <c r="F4" s="44">
+        <v>34763.597999999998</v>
+      </c>
+      <c r="G4" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="46">
+        <f t="shared" ref="H4:H6" si="0">F5*(E4/E5)^2</f>
+        <v>60415.394576000006</v>
+      </c>
+      <c r="I4" s="46">
+        <f>F4</f>
+        <v>34763.597999999998</v>
+      </c>
+      <c r="J4" s="46"/>
+      <c r="K4" s="2">
+        <f>(E4/E5)^2</f>
+        <v>9.6100000000000012</v>
+      </c>
+      <c r="L4" s="50">
+        <f>F4/F5</f>
+        <v>5.5296862517341312</v>
+      </c>
+      <c r="M4" s="49">
+        <f t="shared" ref="M4:M7" si="1">F4/$F$8</f>
+        <v>272.87996722011502</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3.1</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="28">
         <v>916.66660000000002</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="29" t="s">
         <v>21</v>
       </c>
+      <c r="D5" s="29"/>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5" s="40">
+        <v>6286.7215999999999</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="46">
+        <f t="shared" si="0"/>
+        <v>8128.2968000000001</v>
+      </c>
+      <c r="I5" s="46">
+        <f t="shared" ref="I5:I8" si="2">F5</f>
+        <v>6286.7215999999999</v>
+      </c>
+      <c r="J5" s="46"/>
+      <c r="K5" s="2">
+        <f t="shared" ref="K5:K7" si="3">(E5/E6)^2</f>
+        <v>4</v>
+      </c>
+      <c r="L5" s="2">
+        <f>F5/F6</f>
+        <v>3.0937460846656091</v>
+      </c>
+      <c r="M5" s="49">
+        <f t="shared" si="1"/>
+        <v>49.348182663083065</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="28">
         <v>2032.0742</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="29" t="s">
         <v>22</v>
       </c>
+      <c r="D6" s="29"/>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6" s="40">
+        <v>2032.0742</v>
+      </c>
+      <c r="G6" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="46">
+        <f t="shared" si="0"/>
+        <v>2384.6685744016645</v>
+      </c>
+      <c r="I6" s="46">
+        <f t="shared" si="2"/>
+        <v>2032.0742</v>
+      </c>
+      <c r="J6" s="46"/>
+      <c r="K6" s="2">
+        <f t="shared" si="3"/>
+        <v>2.6014568158168569</v>
+      </c>
+      <c r="L6" s="2">
+        <f>F6/F7</f>
+        <v>2.2168083794042457</v>
+      </c>
+      <c r="M6" s="49">
+        <f t="shared" si="1"/>
+        <v>15.950947916405013</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B7" s="28">
         <v>6286.7215999999999</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="29" t="s">
         <v>19</v>
       </c>
+      <c r="D7" s="29"/>
+      <c r="E7">
+        <v>3.1</v>
+      </c>
+      <c r="F7" s="40">
+        <v>916.66660000000002</v>
+      </c>
+      <c r="G7" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="46">
+        <f>F8*(E7/E8)^2</f>
+        <v>1224.2678720000001</v>
+      </c>
+      <c r="I7" s="46">
+        <f t="shared" si="2"/>
+        <v>916.66660000000002</v>
+      </c>
+      <c r="J7" s="46"/>
+      <c r="K7" s="2">
+        <f t="shared" si="3"/>
+        <v>9.6100000000000012</v>
+      </c>
+      <c r="L7" s="2">
+        <f>F7/F8</f>
+        <v>7.1954563437240964</v>
+      </c>
+      <c r="M7" s="49">
+        <f t="shared" si="1"/>
+        <v>7.1954563437240964</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>31</v>
       </c>
-      <c r="B8" s="34">
+      <c r="B8" s="30">
         <v>34763.597999999998</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="29" t="s">
         <v>20</v>
       </c>
+      <c r="D8" s="29"/>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="42">
+        <v>127.3952</v>
+      </c>
+      <c r="G8" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="48">
+        <v>127</v>
+      </c>
+      <c r="I8" s="46">
+        <f t="shared" si="2"/>
+        <v>127.3952</v>
+      </c>
+      <c r="J8" s="46"/>
+      <c r="M8" s="49">
+        <f>F8/$F$8</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K9" s="2">
+        <f>H4/H5</f>
+        <v>7.4327249684091266</v>
+      </c>
+      <c r="L9" s="2">
+        <f>I4/I5</f>
+        <v>5.5296862517341312</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K10" s="2">
+        <f t="shared" ref="K10:L10" si="4">H5/H6</f>
+        <v>3.4085645641719688</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" si="4"/>
+        <v>3.0937460846656091</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K11" s="2">
+        <f t="shared" ref="K11:L11" si="5">H6/H7</f>
+        <v>1.9478323567423195</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" si="5"/>
+        <v>2.2168083794042457</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K12" s="2">
+        <f t="shared" ref="K12" si="6">H7/H8</f>
+        <v>9.639904503937009</v>
+      </c>
+      <c r="L12" s="2">
+        <f t="shared" ref="L12" si="7">I7/I8</f>
+        <v>7.1954563437240964</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -7334,66 +9588,72 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
-      <c r="B14" s="32">
+      <c r="B14" s="28">
         <v>127.3952</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C14" s="28">
         <v>127.3952</v>
       </c>
+      <c r="D14" s="28"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3.1</v>
       </c>
-      <c r="B15" s="32">
+      <c r="B15" s="28">
         <v>916.66660000000002</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="28">
         <v>916.66660000000002</v>
       </c>
+      <c r="D15" s="28"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5</v>
       </c>
-      <c r="B16" s="32">
+      <c r="B16" s="28">
         <v>2032.0742</v>
       </c>
-      <c r="C16" s="32">
+      <c r="C16" s="28">
         <v>2032.0742</v>
       </c>
+      <c r="D16" s="28"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10</v>
       </c>
-      <c r="B17" s="32">
+      <c r="B17" s="28">
         <v>6286.7215999999999</v>
       </c>
-      <c r="C17" s="32">
+      <c r="C17" s="28">
         <v>6286.7215999999999</v>
       </c>
+      <c r="D17" s="28"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>31</v>
       </c>
-      <c r="B18" s="34">
+      <c r="B18" s="30">
         <v>34763.597999999998</v>
       </c>
-      <c r="C18" s="34">
+      <c r="C18" s="30">
         <v>34763.597999999998</v>
       </c>
+      <c r="D18" s="30"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -7404,60 +9664,65 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
-      <c r="B21" s="32">
+      <c r="B21" s="28">
         <v>1</v>
       </c>
-      <c r="C21" s="32">
+      <c r="C21" s="28">
         <v>127.3952</v>
       </c>
+      <c r="D21" s="28"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
-      <c r="C22" s="32">
+      <c r="C22" s="28">
         <v>916.66660000000002</v>
       </c>
+      <c r="D22" s="28"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
-      <c r="C23" s="32">
+      <c r="C23" s="28">
         <v>2032.0742</v>
       </c>
+      <c r="D23" s="28"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
-      <c r="C24" s="32">
+      <c r="C24" s="28">
         <v>6286.7215999999999</v>
       </c>
+      <c r="D24" s="28"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
-      <c r="C25" s="34">
+      <c r="C25" s="30">
         <v>34763.597999999998</v>
       </c>
+      <c r="D25" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>